<commit_message>
Update machine translation papers.xlsx
</commit_message>
<xml_diff>
--- a/papers/machine translation papers.xlsx
+++ b/papers/machine translation papers.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo.saad\Documents\GitHub\machine-translation-master-course\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375C284D-5793-4C8A-9D72-8343CD59F9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7389C7C1-D1AE-40A4-977B-A7B329649D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="6570" windowWidth="15375" windowHeight="7875" xr2:uid="{6CD4D8FD-01DE-4A11-BB66-7FA3939BB517}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
   <si>
     <t>Attention Mechanism</t>
   </si>
@@ -208,6 +209,9 @@
   </si>
   <si>
     <t>Paper</t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
@@ -559,396 +563,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB28102-06EC-438D-8534-DE97E3EBAA27}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="103.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
       <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
       <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
       <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
       <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
       <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
       <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
       <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
       <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B47" xr:uid="{5DB28102-06EC-438D-8534-DE97E3EBAA27}"/>
+  <autoFilter ref="A1:C47" xr:uid="{5DB28102-06EC-438D-8534-DE97E3EBAA27}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0446CE9C-A1AB-4354-9EBC-140ED2D2D512}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>